<commit_message>
SE deliverables toegevoegd voor week 2
</commit_message>
<xml_diff>
--- a/SE Deliverables/Week 2/Sprintplan 2.xlsx
+++ b/SE Deliverables/Week 2/Sprintplan 2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>User Story</t>
   </si>
@@ -31,12 +31,6 @@
   </si>
   <si>
     <t>Estimated Effort per Task</t>
-  </si>
-  <si>
-    <t>Actual Effort per Task (in Hours)</t>
-  </si>
-  <si>
-    <t>Done (yes/no)</t>
   </si>
   <si>
     <t>Notes</t>
@@ -55,9 +49,6 @@
   </si>
   <si>
     <t>Client meeting</t>
-  </si>
-  <si>
-    <t>Task completed by</t>
   </si>
   <si>
     <t>Everybody</t>
@@ -81,16 +72,10 @@
     <t>Place first emotion predicate in GOAL</t>
   </si>
   <si>
-    <t>Contact group 3 (GAM plugin) about GAM and GOAL</t>
-  </si>
-  <si>
     <t>Contact agent and bridge group about relevant percepts</t>
   </si>
   <si>
     <t>Contact other groups about evaluation triggers</t>
-  </si>
-  <si>
-    <t>This week there were only 2 project blocks where we could work on the actual project.</t>
   </si>
   <si>
     <t>Understanding GAM java port</t>
@@ -103,6 +88,27 @@
   </si>
   <si>
     <t>Think about git pull requests</t>
+  </si>
+  <si>
+    <t>Maven en dergelijke opzetten</t>
+  </si>
+  <si>
+    <t>Contact group 4 (GAM plugin) about GAM and GOAL</t>
+  </si>
+  <si>
+    <t>This week there are only 2 project blocks where we can work on the actual project.</t>
+  </si>
+  <si>
+    <t>With TravisCI, Octopull</t>
+  </si>
+  <si>
+    <t>Bernd</t>
+  </si>
+  <si>
+    <t>Rolf</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -276,7 +282,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -313,9 +319,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -335,6 +338,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1668,38 +1677,34 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IX25"/>
+  <dimension ref="A1:IU26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.07421875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="258" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="255" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:258" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+    <row r="1" spans="1:255" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:258" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1710,127 +1715,115 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:255" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="C3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F3" s="4"/>
     </row>
-    <row r="3" spans="1:258" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>4</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:258" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
       <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:258" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
       <c r="E5" s="4">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:258" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
       <c r="E6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:255" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
         <v>1</v>
       </c>
-      <c r="F6" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="F7" s="4"/>
     </row>
-    <row r="7" spans="1:258" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19">
-        <v>2</v>
-      </c>
-      <c r="F7" s="19">
+    <row r="8" spans="1:255" s="12" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="18">
         <v>1</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:258" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="4"/>
+      <c r="E8" s="18">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -2077,30 +2070,17 @@
       <c r="IS8" s="1"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
-      <c r="IV8" s="1"/>
-      <c r="IW8" s="1"/>
-      <c r="IX8" s="1"/>
     </row>
-    <row r="9" spans="1:258" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18">
-        <v>8</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+    <row r="9" spans="1:255" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -2347,725 +2327,947 @@
       <c r="IS9" s="1"/>
       <c r="IT9" s="1"/>
       <c r="IU9" s="1"/>
-      <c r="IV9" s="1"/>
-      <c r="IW9" s="1"/>
-      <c r="IX9" s="1"/>
     </row>
-    <row r="10" spans="1:258" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4">
+    <row r="10" spans="1:255" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="16">
         <v>1</v>
       </c>
-      <c r="F10" s="5">
-        <v>10</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="E10" s="17">
+        <v>8</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+      <c r="BJ10" s="1"/>
+      <c r="BK10" s="1"/>
+      <c r="BL10" s="1"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+      <c r="BQ10" s="1"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+      <c r="BT10" s="1"/>
+      <c r="BU10" s="1"/>
+      <c r="BV10" s="1"/>
+      <c r="BW10" s="1"/>
+      <c r="BX10" s="1"/>
+      <c r="BY10" s="1"/>
+      <c r="BZ10" s="1"/>
+      <c r="CA10" s="1"/>
+      <c r="CB10" s="1"/>
+      <c r="CC10" s="1"/>
+      <c r="CD10" s="1"/>
+      <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
+      <c r="CG10" s="1"/>
+      <c r="CH10" s="1"/>
+      <c r="CI10" s="1"/>
+      <c r="CJ10" s="1"/>
+      <c r="CK10" s="1"/>
+      <c r="CL10" s="1"/>
+      <c r="CM10" s="1"/>
+      <c r="CN10" s="1"/>
+      <c r="CO10" s="1"/>
+      <c r="CP10" s="1"/>
+      <c r="CQ10" s="1"/>
+      <c r="CR10" s="1"/>
+      <c r="CS10" s="1"/>
+      <c r="CT10" s="1"/>
+      <c r="CU10" s="1"/>
+      <c r="CV10" s="1"/>
+      <c r="CW10" s="1"/>
+      <c r="CX10" s="1"/>
+      <c r="CY10" s="1"/>
+      <c r="CZ10" s="1"/>
+      <c r="DA10" s="1"/>
+      <c r="DB10" s="1"/>
+      <c r="DC10" s="1"/>
+      <c r="DD10" s="1"/>
+      <c r="DE10" s="1"/>
+      <c r="DF10" s="1"/>
+      <c r="DG10" s="1"/>
+      <c r="DH10" s="1"/>
+      <c r="DI10" s="1"/>
+      <c r="DJ10" s="1"/>
+      <c r="DK10" s="1"/>
+      <c r="DL10" s="1"/>
+      <c r="DM10" s="1"/>
+      <c r="DN10" s="1"/>
+      <c r="DO10" s="1"/>
+      <c r="DP10" s="1"/>
+      <c r="DQ10" s="1"/>
+      <c r="DR10" s="1"/>
+      <c r="DS10" s="1"/>
+      <c r="DT10" s="1"/>
+      <c r="DU10" s="1"/>
+      <c r="DV10" s="1"/>
+      <c r="DW10" s="1"/>
+      <c r="DX10" s="1"/>
+      <c r="DY10" s="1"/>
+      <c r="DZ10" s="1"/>
+      <c r="EA10" s="1"/>
+      <c r="EB10" s="1"/>
+      <c r="EC10" s="1"/>
+      <c r="ED10" s="1"/>
+      <c r="EE10" s="1"/>
+      <c r="EF10" s="1"/>
+      <c r="EG10" s="1"/>
+      <c r="EH10" s="1"/>
+      <c r="EI10" s="1"/>
+      <c r="EJ10" s="1"/>
+      <c r="EK10" s="1"/>
+      <c r="EL10" s="1"/>
+      <c r="EM10" s="1"/>
+      <c r="EN10" s="1"/>
+      <c r="EO10" s="1"/>
+      <c r="EP10" s="1"/>
+      <c r="EQ10" s="1"/>
+      <c r="ER10" s="1"/>
+      <c r="ES10" s="1"/>
+      <c r="ET10" s="1"/>
+      <c r="EU10" s="1"/>
+      <c r="EV10" s="1"/>
+      <c r="EW10" s="1"/>
+      <c r="EX10" s="1"/>
+      <c r="EY10" s="1"/>
+      <c r="EZ10" s="1"/>
+      <c r="FA10" s="1"/>
+      <c r="FB10" s="1"/>
+      <c r="FC10" s="1"/>
+      <c r="FD10" s="1"/>
+      <c r="FE10" s="1"/>
+      <c r="FF10" s="1"/>
+      <c r="FG10" s="1"/>
+      <c r="FH10" s="1"/>
+      <c r="FI10" s="1"/>
+      <c r="FJ10" s="1"/>
+      <c r="FK10" s="1"/>
+      <c r="FL10" s="1"/>
+      <c r="FM10" s="1"/>
+      <c r="FN10" s="1"/>
+      <c r="FO10" s="1"/>
+      <c r="FP10" s="1"/>
+      <c r="FQ10" s="1"/>
+      <c r="FR10" s="1"/>
+      <c r="FS10" s="1"/>
+      <c r="FT10" s="1"/>
+      <c r="FU10" s="1"/>
+      <c r="FV10" s="1"/>
+      <c r="FW10" s="1"/>
+      <c r="FX10" s="1"/>
+      <c r="FY10" s="1"/>
+      <c r="FZ10" s="1"/>
+      <c r="GA10" s="1"/>
+      <c r="GB10" s="1"/>
+      <c r="GC10" s="1"/>
+      <c r="GD10" s="1"/>
+      <c r="GE10" s="1"/>
+      <c r="GF10" s="1"/>
+      <c r="GG10" s="1"/>
+      <c r="GH10" s="1"/>
+      <c r="GI10" s="1"/>
+      <c r="GJ10" s="1"/>
+      <c r="GK10" s="1"/>
+      <c r="GL10" s="1"/>
+      <c r="GM10" s="1"/>
+      <c r="GN10" s="1"/>
+      <c r="GO10" s="1"/>
+      <c r="GP10" s="1"/>
+      <c r="GQ10" s="1"/>
+      <c r="GR10" s="1"/>
+      <c r="GS10" s="1"/>
+      <c r="GT10" s="1"/>
+      <c r="GU10" s="1"/>
+      <c r="GV10" s="1"/>
+      <c r="GW10" s="1"/>
+      <c r="GX10" s="1"/>
+      <c r="GY10" s="1"/>
+      <c r="GZ10" s="1"/>
+      <c r="HA10" s="1"/>
+      <c r="HB10" s="1"/>
+      <c r="HC10" s="1"/>
+      <c r="HD10" s="1"/>
+      <c r="HE10" s="1"/>
+      <c r="HF10" s="1"/>
+      <c r="HG10" s="1"/>
+      <c r="HH10" s="1"/>
+      <c r="HI10" s="1"/>
+      <c r="HJ10" s="1"/>
+      <c r="HK10" s="1"/>
+      <c r="HL10" s="1"/>
+      <c r="HM10" s="1"/>
+      <c r="HN10" s="1"/>
+      <c r="HO10" s="1"/>
+      <c r="HP10" s="1"/>
+      <c r="HQ10" s="1"/>
+      <c r="HR10" s="1"/>
+      <c r="HS10" s="1"/>
+      <c r="HT10" s="1"/>
+      <c r="HU10" s="1"/>
+      <c r="HV10" s="1"/>
+      <c r="HW10" s="1"/>
+      <c r="HX10" s="1"/>
+      <c r="HY10" s="1"/>
+      <c r="HZ10" s="1"/>
+      <c r="IA10" s="1"/>
+      <c r="IB10" s="1"/>
+      <c r="IC10" s="1"/>
+      <c r="ID10" s="1"/>
+      <c r="IE10" s="1"/>
+      <c r="IF10" s="1"/>
+      <c r="IG10" s="1"/>
+      <c r="IH10" s="1"/>
+      <c r="II10" s="1"/>
+      <c r="IJ10" s="1"/>
+      <c r="IK10" s="1"/>
+      <c r="IL10" s="1"/>
+      <c r="IM10" s="1"/>
+      <c r="IN10" s="1"/>
+      <c r="IO10" s="1"/>
+      <c r="IP10" s="1"/>
+      <c r="IQ10" s="1"/>
+      <c r="IR10" s="1"/>
+      <c r="IS10" s="1"/>
+      <c r="IT10" s="1"/>
+      <c r="IU10" s="1"/>
     </row>
-    <row r="11" spans="1:258" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:255" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
-        <v>2</v>
-      </c>
-      <c r="F11" s="4">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:258" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:255" s="9" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="1"/>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+      <c r="BO14" s="1"/>
+      <c r="BP14" s="1"/>
+      <c r="BQ14" s="1"/>
+      <c r="BR14" s="1"/>
+      <c r="BS14" s="1"/>
+      <c r="BT14" s="1"/>
+      <c r="BU14" s="1"/>
+      <c r="BV14" s="1"/>
+      <c r="BW14" s="1"/>
+      <c r="BX14" s="1"/>
+      <c r="BY14" s="1"/>
+      <c r="BZ14" s="1"/>
+      <c r="CA14" s="1"/>
+      <c r="CB14" s="1"/>
+      <c r="CC14" s="1"/>
+      <c r="CD14" s="1"/>
+      <c r="CE14" s="1"/>
+      <c r="CF14" s="1"/>
+      <c r="CG14" s="1"/>
+      <c r="CH14" s="1"/>
+      <c r="CI14" s="1"/>
+      <c r="CJ14" s="1"/>
+      <c r="CK14" s="1"/>
+      <c r="CL14" s="1"/>
+      <c r="CM14" s="1"/>
+      <c r="CN14" s="1"/>
+      <c r="CO14" s="1"/>
+      <c r="CP14" s="1"/>
+      <c r="CQ14" s="1"/>
+      <c r="CR14" s="1"/>
+      <c r="CS14" s="1"/>
+      <c r="CT14" s="1"/>
+      <c r="CU14" s="1"/>
+      <c r="CV14" s="1"/>
+      <c r="CW14" s="1"/>
+      <c r="CX14" s="1"/>
+      <c r="CY14" s="1"/>
+      <c r="CZ14" s="1"/>
+      <c r="DA14" s="1"/>
+      <c r="DB14" s="1"/>
+      <c r="DC14" s="1"/>
+      <c r="DD14" s="1"/>
+      <c r="DE14" s="1"/>
+      <c r="DF14" s="1"/>
+      <c r="DG14" s="1"/>
+      <c r="DH14" s="1"/>
+      <c r="DI14" s="1"/>
+      <c r="DJ14" s="1"/>
+      <c r="DK14" s="1"/>
+      <c r="DL14" s="1"/>
+      <c r="DM14" s="1"/>
+      <c r="DN14" s="1"/>
+      <c r="DO14" s="1"/>
+      <c r="DP14" s="1"/>
+      <c r="DQ14" s="1"/>
+      <c r="DR14" s="1"/>
+      <c r="DS14" s="1"/>
+      <c r="DT14" s="1"/>
+      <c r="DU14" s="1"/>
+      <c r="DV14" s="1"/>
+      <c r="DW14" s="1"/>
+      <c r="DX14" s="1"/>
+      <c r="DY14" s="1"/>
+      <c r="DZ14" s="1"/>
+      <c r="EA14" s="1"/>
+      <c r="EB14" s="1"/>
+      <c r="EC14" s="1"/>
+      <c r="ED14" s="1"/>
+      <c r="EE14" s="1"/>
+      <c r="EF14" s="1"/>
+      <c r="EG14" s="1"/>
+      <c r="EH14" s="1"/>
+      <c r="EI14" s="1"/>
+      <c r="EJ14" s="1"/>
+      <c r="EK14" s="1"/>
+      <c r="EL14" s="1"/>
+      <c r="EM14" s="1"/>
+      <c r="EN14" s="1"/>
+      <c r="EO14" s="1"/>
+      <c r="EP14" s="1"/>
+      <c r="EQ14" s="1"/>
+      <c r="ER14" s="1"/>
+      <c r="ES14" s="1"/>
+      <c r="ET14" s="1"/>
+      <c r="EU14" s="1"/>
+      <c r="EV14" s="1"/>
+      <c r="EW14" s="1"/>
+      <c r="EX14" s="1"/>
+      <c r="EY14" s="1"/>
+      <c r="EZ14" s="1"/>
+      <c r="FA14" s="1"/>
+      <c r="FB14" s="1"/>
+      <c r="FC14" s="1"/>
+      <c r="FD14" s="1"/>
+      <c r="FE14" s="1"/>
+      <c r="FF14" s="1"/>
+      <c r="FG14" s="1"/>
+      <c r="FH14" s="1"/>
+      <c r="FI14" s="1"/>
+      <c r="FJ14" s="1"/>
+      <c r="FK14" s="1"/>
+      <c r="FL14" s="1"/>
+      <c r="FM14" s="1"/>
+      <c r="FN14" s="1"/>
+      <c r="FO14" s="1"/>
+      <c r="FP14" s="1"/>
+      <c r="FQ14" s="1"/>
+      <c r="FR14" s="1"/>
+      <c r="FS14" s="1"/>
+      <c r="FT14" s="1"/>
+      <c r="FU14" s="1"/>
+      <c r="FV14" s="1"/>
+      <c r="FW14" s="1"/>
+      <c r="FX14" s="1"/>
+      <c r="FY14" s="1"/>
+      <c r="FZ14" s="1"/>
+      <c r="GA14" s="1"/>
+      <c r="GB14" s="1"/>
+      <c r="GC14" s="1"/>
+      <c r="GD14" s="1"/>
+      <c r="GE14" s="1"/>
+      <c r="GF14" s="1"/>
+      <c r="GG14" s="1"/>
+      <c r="GH14" s="1"/>
+      <c r="GI14" s="1"/>
+      <c r="GJ14" s="1"/>
+      <c r="GK14" s="1"/>
+      <c r="GL14" s="1"/>
+      <c r="GM14" s="1"/>
+      <c r="GN14" s="1"/>
+      <c r="GO14" s="1"/>
+      <c r="GP14" s="1"/>
+      <c r="GQ14" s="1"/>
+      <c r="GR14" s="1"/>
+      <c r="GS14" s="1"/>
+      <c r="GT14" s="1"/>
+      <c r="GU14" s="1"/>
+      <c r="GV14" s="1"/>
+      <c r="GW14" s="1"/>
+      <c r="GX14" s="1"/>
+      <c r="GY14" s="1"/>
+      <c r="GZ14" s="1"/>
+      <c r="HA14" s="1"/>
+      <c r="HB14" s="1"/>
+      <c r="HC14" s="1"/>
+      <c r="HD14" s="1"/>
+      <c r="HE14" s="1"/>
+      <c r="HF14" s="1"/>
+      <c r="HG14" s="1"/>
+      <c r="HH14" s="1"/>
+      <c r="HI14" s="1"/>
+      <c r="HJ14" s="1"/>
+      <c r="HK14" s="1"/>
+      <c r="HL14" s="1"/>
+      <c r="HM14" s="1"/>
+      <c r="HN14" s="1"/>
+      <c r="HO14" s="1"/>
+      <c r="HP14" s="1"/>
+      <c r="HQ14" s="1"/>
+      <c r="HR14" s="1"/>
+      <c r="HS14" s="1"/>
+      <c r="HT14" s="1"/>
+      <c r="HU14" s="1"/>
+      <c r="HV14" s="1"/>
+      <c r="HW14" s="1"/>
+      <c r="HX14" s="1"/>
+      <c r="HY14" s="1"/>
+      <c r="HZ14" s="1"/>
+      <c r="IA14" s="1"/>
+      <c r="IB14" s="1"/>
+      <c r="IC14" s="1"/>
+      <c r="ID14" s="1"/>
+      <c r="IE14" s="1"/>
+      <c r="IF14" s="1"/>
+      <c r="IG14" s="1"/>
+      <c r="IH14" s="1"/>
+      <c r="II14" s="1"/>
+      <c r="IJ14" s="1"/>
+      <c r="IK14" s="1"/>
+      <c r="IL14" s="1"/>
+      <c r="IM14" s="1"/>
+      <c r="IN14" s="1"/>
+      <c r="IO14" s="1"/>
+      <c r="IP14" s="1"/>
+      <c r="IQ14" s="1"/>
+      <c r="IR14" s="1"/>
+      <c r="IS14" s="1"/>
+      <c r="IT14" s="1"/>
+      <c r="IU14" s="1"/>
+    </row>
+    <row r="15" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4"/>
     </row>
-    <row r="13" spans="1:258" s="9" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="1"/>
-      <c r="AT13" s="1"/>
-      <c r="AU13" s="1"/>
-      <c r="AV13" s="1"/>
-      <c r="AW13" s="1"/>
-      <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
-      <c r="AZ13" s="1"/>
-      <c r="BA13" s="1"/>
-      <c r="BB13" s="1"/>
-      <c r="BC13" s="1"/>
-      <c r="BD13" s="1"/>
-      <c r="BE13" s="1"/>
-      <c r="BF13" s="1"/>
-      <c r="BG13" s="1"/>
-      <c r="BH13" s="1"/>
-      <c r="BI13" s="1"/>
-      <c r="BJ13" s="1"/>
-      <c r="BK13" s="1"/>
-      <c r="BL13" s="1"/>
-      <c r="BM13" s="1"/>
-      <c r="BN13" s="1"/>
-      <c r="BO13" s="1"/>
-      <c r="BP13" s="1"/>
-      <c r="BQ13" s="1"/>
-      <c r="BR13" s="1"/>
-      <c r="BS13" s="1"/>
-      <c r="BT13" s="1"/>
-      <c r="BU13" s="1"/>
-      <c r="BV13" s="1"/>
-      <c r="BW13" s="1"/>
-      <c r="BX13" s="1"/>
-      <c r="BY13" s="1"/>
-      <c r="BZ13" s="1"/>
-      <c r="CA13" s="1"/>
-      <c r="CB13" s="1"/>
-      <c r="CC13" s="1"/>
-      <c r="CD13" s="1"/>
-      <c r="CE13" s="1"/>
-      <c r="CF13" s="1"/>
-      <c r="CG13" s="1"/>
-      <c r="CH13" s="1"/>
-      <c r="CI13" s="1"/>
-      <c r="CJ13" s="1"/>
-      <c r="CK13" s="1"/>
-      <c r="CL13" s="1"/>
-      <c r="CM13" s="1"/>
-      <c r="CN13" s="1"/>
-      <c r="CO13" s="1"/>
-      <c r="CP13" s="1"/>
-      <c r="CQ13" s="1"/>
-      <c r="CR13" s="1"/>
-      <c r="CS13" s="1"/>
-      <c r="CT13" s="1"/>
-      <c r="CU13" s="1"/>
-      <c r="CV13" s="1"/>
-      <c r="CW13" s="1"/>
-      <c r="CX13" s="1"/>
-      <c r="CY13" s="1"/>
-      <c r="CZ13" s="1"/>
-      <c r="DA13" s="1"/>
-      <c r="DB13" s="1"/>
-      <c r="DC13" s="1"/>
-      <c r="DD13" s="1"/>
-      <c r="DE13" s="1"/>
-      <c r="DF13" s="1"/>
-      <c r="DG13" s="1"/>
-      <c r="DH13" s="1"/>
-      <c r="DI13" s="1"/>
-      <c r="DJ13" s="1"/>
-      <c r="DK13" s="1"/>
-      <c r="DL13" s="1"/>
-      <c r="DM13" s="1"/>
-      <c r="DN13" s="1"/>
-      <c r="DO13" s="1"/>
-      <c r="DP13" s="1"/>
-      <c r="DQ13" s="1"/>
-      <c r="DR13" s="1"/>
-      <c r="DS13" s="1"/>
-      <c r="DT13" s="1"/>
-      <c r="DU13" s="1"/>
-      <c r="DV13" s="1"/>
-      <c r="DW13" s="1"/>
-      <c r="DX13" s="1"/>
-      <c r="DY13" s="1"/>
-      <c r="DZ13" s="1"/>
-      <c r="EA13" s="1"/>
-      <c r="EB13" s="1"/>
-      <c r="EC13" s="1"/>
-      <c r="ED13" s="1"/>
-      <c r="EE13" s="1"/>
-      <c r="EF13" s="1"/>
-      <c r="EG13" s="1"/>
-      <c r="EH13" s="1"/>
-      <c r="EI13" s="1"/>
-      <c r="EJ13" s="1"/>
-      <c r="EK13" s="1"/>
-      <c r="EL13" s="1"/>
-      <c r="EM13" s="1"/>
-      <c r="EN13" s="1"/>
-      <c r="EO13" s="1"/>
-      <c r="EP13" s="1"/>
-      <c r="EQ13" s="1"/>
-      <c r="ER13" s="1"/>
-      <c r="ES13" s="1"/>
-      <c r="ET13" s="1"/>
-      <c r="EU13" s="1"/>
-      <c r="EV13" s="1"/>
-      <c r="EW13" s="1"/>
-      <c r="EX13" s="1"/>
-      <c r="EY13" s="1"/>
-      <c r="EZ13" s="1"/>
-      <c r="FA13" s="1"/>
-      <c r="FB13" s="1"/>
-      <c r="FC13" s="1"/>
-      <c r="FD13" s="1"/>
-      <c r="FE13" s="1"/>
-      <c r="FF13" s="1"/>
-      <c r="FG13" s="1"/>
-      <c r="FH13" s="1"/>
-      <c r="FI13" s="1"/>
-      <c r="FJ13" s="1"/>
-      <c r="FK13" s="1"/>
-      <c r="FL13" s="1"/>
-      <c r="FM13" s="1"/>
-      <c r="FN13" s="1"/>
-      <c r="FO13" s="1"/>
-      <c r="FP13" s="1"/>
-      <c r="FQ13" s="1"/>
-      <c r="FR13" s="1"/>
-      <c r="FS13" s="1"/>
-      <c r="FT13" s="1"/>
-      <c r="FU13" s="1"/>
-      <c r="FV13" s="1"/>
-      <c r="FW13" s="1"/>
-      <c r="FX13" s="1"/>
-      <c r="FY13" s="1"/>
-      <c r="FZ13" s="1"/>
-      <c r="GA13" s="1"/>
-      <c r="GB13" s="1"/>
-      <c r="GC13" s="1"/>
-      <c r="GD13" s="1"/>
-      <c r="GE13" s="1"/>
-      <c r="GF13" s="1"/>
-      <c r="GG13" s="1"/>
-      <c r="GH13" s="1"/>
-      <c r="GI13" s="1"/>
-      <c r="GJ13" s="1"/>
-      <c r="GK13" s="1"/>
-      <c r="GL13" s="1"/>
-      <c r="GM13" s="1"/>
-      <c r="GN13" s="1"/>
-      <c r="GO13" s="1"/>
-      <c r="GP13" s="1"/>
-      <c r="GQ13" s="1"/>
-      <c r="GR13" s="1"/>
-      <c r="GS13" s="1"/>
-      <c r="GT13" s="1"/>
-      <c r="GU13" s="1"/>
-      <c r="GV13" s="1"/>
-      <c r="GW13" s="1"/>
-      <c r="GX13" s="1"/>
-      <c r="GY13" s="1"/>
-      <c r="GZ13" s="1"/>
-      <c r="HA13" s="1"/>
-      <c r="HB13" s="1"/>
-      <c r="HC13" s="1"/>
-      <c r="HD13" s="1"/>
-      <c r="HE13" s="1"/>
-      <c r="HF13" s="1"/>
-      <c r="HG13" s="1"/>
-      <c r="HH13" s="1"/>
-      <c r="HI13" s="1"/>
-      <c r="HJ13" s="1"/>
-      <c r="HK13" s="1"/>
-      <c r="HL13" s="1"/>
-      <c r="HM13" s="1"/>
-      <c r="HN13" s="1"/>
-      <c r="HO13" s="1"/>
-      <c r="HP13" s="1"/>
-      <c r="HQ13" s="1"/>
-      <c r="HR13" s="1"/>
-      <c r="HS13" s="1"/>
-      <c r="HT13" s="1"/>
-      <c r="HU13" s="1"/>
-      <c r="HV13" s="1"/>
-      <c r="HW13" s="1"/>
-      <c r="HX13" s="1"/>
-      <c r="HY13" s="1"/>
-      <c r="HZ13" s="1"/>
-      <c r="IA13" s="1"/>
-      <c r="IB13" s="1"/>
-      <c r="IC13" s="1"/>
-      <c r="ID13" s="1"/>
-      <c r="IE13" s="1"/>
-      <c r="IF13" s="1"/>
-      <c r="IG13" s="1"/>
-      <c r="IH13" s="1"/>
-      <c r="II13" s="1"/>
-      <c r="IJ13" s="1"/>
-      <c r="IK13" s="1"/>
-      <c r="IL13" s="1"/>
-      <c r="IM13" s="1"/>
-      <c r="IN13" s="1"/>
-      <c r="IO13" s="1"/>
-      <c r="IP13" s="1"/>
-      <c r="IQ13" s="1"/>
-      <c r="IR13" s="1"/>
-      <c r="IS13" s="1"/>
-      <c r="IT13" s="1"/>
-      <c r="IU13" s="1"/>
-      <c r="IV13" s="1"/>
-      <c r="IW13" s="1"/>
-      <c r="IX13" s="1"/>
-    </row>
-    <row r="14" spans="1:258" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>4</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:258" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>4</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:258" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
-      <c r="AJ16" s="1"/>
-      <c r="AK16" s="1"/>
-      <c r="AL16" s="1"/>
-      <c r="AM16" s="1"/>
-      <c r="AN16" s="1"/>
-      <c r="AO16" s="1"/>
-      <c r="AP16" s="1"/>
-      <c r="AQ16" s="1"/>
-      <c r="AR16" s="1"/>
-      <c r="AS16" s="1"/>
-      <c r="AT16" s="1"/>
-      <c r="AU16" s="1"/>
-      <c r="AV16" s="1"/>
-      <c r="AW16" s="1"/>
-      <c r="AX16" s="1"/>
-      <c r="AY16" s="1"/>
-      <c r="AZ16" s="1"/>
-      <c r="BA16" s="1"/>
-      <c r="BB16" s="1"/>
-      <c r="BC16" s="1"/>
-      <c r="BD16" s="1"/>
-      <c r="BE16" s="1"/>
-      <c r="BF16" s="1"/>
-      <c r="BG16" s="1"/>
-      <c r="BH16" s="1"/>
-      <c r="BI16" s="1"/>
-      <c r="BJ16" s="1"/>
-      <c r="BK16" s="1"/>
-      <c r="BL16" s="1"/>
-      <c r="BM16" s="1"/>
-      <c r="BN16" s="1"/>
-      <c r="BO16" s="1"/>
-      <c r="BP16" s="1"/>
-      <c r="BQ16" s="1"/>
-      <c r="BR16" s="1"/>
-      <c r="BS16" s="1"/>
-      <c r="BT16" s="1"/>
-      <c r="BU16" s="1"/>
-      <c r="BV16" s="1"/>
-      <c r="BW16" s="1"/>
-      <c r="BX16" s="1"/>
-      <c r="BY16" s="1"/>
-      <c r="BZ16" s="1"/>
-      <c r="CA16" s="1"/>
-      <c r="CB16" s="1"/>
-      <c r="CC16" s="1"/>
-      <c r="CD16" s="1"/>
-      <c r="CE16" s="1"/>
-      <c r="CF16" s="1"/>
-      <c r="CG16" s="1"/>
-      <c r="CH16" s="1"/>
-      <c r="CI16" s="1"/>
-      <c r="CJ16" s="1"/>
-      <c r="CK16" s="1"/>
-      <c r="CL16" s="1"/>
-      <c r="CM16" s="1"/>
-      <c r="CN16" s="1"/>
-      <c r="CO16" s="1"/>
-      <c r="CP16" s="1"/>
-      <c r="CQ16" s="1"/>
-      <c r="CR16" s="1"/>
-      <c r="CS16" s="1"/>
-      <c r="CT16" s="1"/>
-      <c r="CU16" s="1"/>
-      <c r="CV16" s="1"/>
-      <c r="CW16" s="1"/>
-      <c r="CX16" s="1"/>
-      <c r="CY16" s="1"/>
-      <c r="CZ16" s="1"/>
-      <c r="DA16" s="1"/>
-      <c r="DB16" s="1"/>
-      <c r="DC16" s="1"/>
-      <c r="DD16" s="1"/>
-      <c r="DE16" s="1"/>
-      <c r="DF16" s="1"/>
-      <c r="DG16" s="1"/>
-      <c r="DH16" s="1"/>
-      <c r="DI16" s="1"/>
-      <c r="DJ16" s="1"/>
-      <c r="DK16" s="1"/>
-      <c r="DL16" s="1"/>
-      <c r="DM16" s="1"/>
-      <c r="DN16" s="1"/>
-      <c r="DO16" s="1"/>
-      <c r="DP16" s="1"/>
-      <c r="DQ16" s="1"/>
-      <c r="DR16" s="1"/>
-      <c r="DS16" s="1"/>
-      <c r="DT16" s="1"/>
-      <c r="DU16" s="1"/>
-      <c r="DV16" s="1"/>
-      <c r="DW16" s="1"/>
-      <c r="DX16" s="1"/>
-      <c r="DY16" s="1"/>
-      <c r="DZ16" s="1"/>
-      <c r="EA16" s="1"/>
-      <c r="EB16" s="1"/>
-      <c r="EC16" s="1"/>
-      <c r="ED16" s="1"/>
-      <c r="EE16" s="1"/>
-      <c r="EF16" s="1"/>
-      <c r="EG16" s="1"/>
-      <c r="EH16" s="1"/>
-      <c r="EI16" s="1"/>
-      <c r="EJ16" s="1"/>
-      <c r="EK16" s="1"/>
-      <c r="EL16" s="1"/>
-      <c r="EM16" s="1"/>
-      <c r="EN16" s="1"/>
-      <c r="EO16" s="1"/>
-      <c r="EP16" s="1"/>
-      <c r="EQ16" s="1"/>
-      <c r="ER16" s="1"/>
-      <c r="ES16" s="1"/>
-      <c r="ET16" s="1"/>
-      <c r="EU16" s="1"/>
-      <c r="EV16" s="1"/>
-      <c r="EW16" s="1"/>
-      <c r="EX16" s="1"/>
-      <c r="EY16" s="1"/>
-      <c r="EZ16" s="1"/>
-      <c r="FA16" s="1"/>
-      <c r="FB16" s="1"/>
-      <c r="FC16" s="1"/>
-      <c r="FD16" s="1"/>
-      <c r="FE16" s="1"/>
-      <c r="FF16" s="1"/>
-      <c r="FG16" s="1"/>
-      <c r="FH16" s="1"/>
-      <c r="FI16" s="1"/>
-      <c r="FJ16" s="1"/>
-      <c r="FK16" s="1"/>
-      <c r="FL16" s="1"/>
-      <c r="FM16" s="1"/>
-      <c r="FN16" s="1"/>
-      <c r="FO16" s="1"/>
-      <c r="FP16" s="1"/>
-      <c r="FQ16" s="1"/>
-      <c r="FR16" s="1"/>
-      <c r="FS16" s="1"/>
-      <c r="FT16" s="1"/>
-      <c r="FU16" s="1"/>
-      <c r="FV16" s="1"/>
-      <c r="FW16" s="1"/>
-      <c r="FX16" s="1"/>
-      <c r="FY16" s="1"/>
-      <c r="FZ16" s="1"/>
-      <c r="GA16" s="1"/>
-      <c r="GB16" s="1"/>
-      <c r="GC16" s="1"/>
-      <c r="GD16" s="1"/>
-      <c r="GE16" s="1"/>
-      <c r="GF16" s="1"/>
-      <c r="GG16" s="1"/>
-      <c r="GH16" s="1"/>
-      <c r="GI16" s="1"/>
-      <c r="GJ16" s="1"/>
-      <c r="GK16" s="1"/>
-      <c r="GL16" s="1"/>
-      <c r="GM16" s="1"/>
-      <c r="GN16" s="1"/>
-      <c r="GO16" s="1"/>
-      <c r="GP16" s="1"/>
-      <c r="GQ16" s="1"/>
-      <c r="GR16" s="1"/>
-      <c r="GS16" s="1"/>
-      <c r="GT16" s="1"/>
-      <c r="GU16" s="1"/>
-      <c r="GV16" s="1"/>
-      <c r="GW16" s="1"/>
-      <c r="GX16" s="1"/>
-      <c r="GY16" s="1"/>
-      <c r="GZ16" s="1"/>
-      <c r="HA16" s="1"/>
-      <c r="HB16" s="1"/>
-      <c r="HC16" s="1"/>
-      <c r="HD16" s="1"/>
-      <c r="HE16" s="1"/>
-      <c r="HF16" s="1"/>
-      <c r="HG16" s="1"/>
-      <c r="HH16" s="1"/>
-      <c r="HI16" s="1"/>
-      <c r="HJ16" s="1"/>
-      <c r="HK16" s="1"/>
-      <c r="HL16" s="1"/>
-      <c r="HM16" s="1"/>
-      <c r="HN16" s="1"/>
-      <c r="HO16" s="1"/>
-      <c r="HP16" s="1"/>
-      <c r="HQ16" s="1"/>
-      <c r="HR16" s="1"/>
-      <c r="HS16" s="1"/>
-      <c r="HT16" s="1"/>
-      <c r="HU16" s="1"/>
-      <c r="HV16" s="1"/>
-      <c r="HW16" s="1"/>
-      <c r="HX16" s="1"/>
-      <c r="HY16" s="1"/>
-      <c r="HZ16" s="1"/>
-      <c r="IA16" s="1"/>
-      <c r="IB16" s="1"/>
-      <c r="IC16" s="1"/>
-      <c r="ID16" s="1"/>
-      <c r="IE16" s="1"/>
-      <c r="IF16" s="1"/>
-      <c r="IG16" s="1"/>
-      <c r="IH16" s="1"/>
-      <c r="II16" s="1"/>
-      <c r="IJ16" s="1"/>
-      <c r="IK16" s="1"/>
-      <c r="IL16" s="1"/>
-      <c r="IM16" s="1"/>
-      <c r="IN16" s="1"/>
-      <c r="IO16" s="1"/>
-      <c r="IP16" s="1"/>
-      <c r="IQ16" s="1"/>
-      <c r="IR16" s="1"/>
-      <c r="IS16" s="1"/>
-      <c r="IT16" s="1"/>
-      <c r="IU16" s="1"/>
-      <c r="IV16" s="1"/>
-      <c r="IW16" s="1"/>
-      <c r="IX16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:255" s="9" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+      <c r="BP17" s="1"/>
+      <c r="BQ17" s="1"/>
+      <c r="BR17" s="1"/>
+      <c r="BS17" s="1"/>
+      <c r="BT17" s="1"/>
+      <c r="BU17" s="1"/>
+      <c r="BV17" s="1"/>
+      <c r="BW17" s="1"/>
+      <c r="BX17" s="1"/>
+      <c r="BY17" s="1"/>
+      <c r="BZ17" s="1"/>
+      <c r="CA17" s="1"/>
+      <c r="CB17" s="1"/>
+      <c r="CC17" s="1"/>
+      <c r="CD17" s="1"/>
+      <c r="CE17" s="1"/>
+      <c r="CF17" s="1"/>
+      <c r="CG17" s="1"/>
+      <c r="CH17" s="1"/>
+      <c r="CI17" s="1"/>
+      <c r="CJ17" s="1"/>
+      <c r="CK17" s="1"/>
+      <c r="CL17" s="1"/>
+      <c r="CM17" s="1"/>
+      <c r="CN17" s="1"/>
+      <c r="CO17" s="1"/>
+      <c r="CP17" s="1"/>
+      <c r="CQ17" s="1"/>
+      <c r="CR17" s="1"/>
+      <c r="CS17" s="1"/>
+      <c r="CT17" s="1"/>
+      <c r="CU17" s="1"/>
+      <c r="CV17" s="1"/>
+      <c r="CW17" s="1"/>
+      <c r="CX17" s="1"/>
+      <c r="CY17" s="1"/>
+      <c r="CZ17" s="1"/>
+      <c r="DA17" s="1"/>
+      <c r="DB17" s="1"/>
+      <c r="DC17" s="1"/>
+      <c r="DD17" s="1"/>
+      <c r="DE17" s="1"/>
+      <c r="DF17" s="1"/>
+      <c r="DG17" s="1"/>
+      <c r="DH17" s="1"/>
+      <c r="DI17" s="1"/>
+      <c r="DJ17" s="1"/>
+      <c r="DK17" s="1"/>
+      <c r="DL17" s="1"/>
+      <c r="DM17" s="1"/>
+      <c r="DN17" s="1"/>
+      <c r="DO17" s="1"/>
+      <c r="DP17" s="1"/>
+      <c r="DQ17" s="1"/>
+      <c r="DR17" s="1"/>
+      <c r="DS17" s="1"/>
+      <c r="DT17" s="1"/>
+      <c r="DU17" s="1"/>
+      <c r="DV17" s="1"/>
+      <c r="DW17" s="1"/>
+      <c r="DX17" s="1"/>
+      <c r="DY17" s="1"/>
+      <c r="DZ17" s="1"/>
+      <c r="EA17" s="1"/>
+      <c r="EB17" s="1"/>
+      <c r="EC17" s="1"/>
+      <c r="ED17" s="1"/>
+      <c r="EE17" s="1"/>
+      <c r="EF17" s="1"/>
+      <c r="EG17" s="1"/>
+      <c r="EH17" s="1"/>
+      <c r="EI17" s="1"/>
+      <c r="EJ17" s="1"/>
+      <c r="EK17" s="1"/>
+      <c r="EL17" s="1"/>
+      <c r="EM17" s="1"/>
+      <c r="EN17" s="1"/>
+      <c r="EO17" s="1"/>
+      <c r="EP17" s="1"/>
+      <c r="EQ17" s="1"/>
+      <c r="ER17" s="1"/>
+      <c r="ES17" s="1"/>
+      <c r="ET17" s="1"/>
+      <c r="EU17" s="1"/>
+      <c r="EV17" s="1"/>
+      <c r="EW17" s="1"/>
+      <c r="EX17" s="1"/>
+      <c r="EY17" s="1"/>
+      <c r="EZ17" s="1"/>
+      <c r="FA17" s="1"/>
+      <c r="FB17" s="1"/>
+      <c r="FC17" s="1"/>
+      <c r="FD17" s="1"/>
+      <c r="FE17" s="1"/>
+      <c r="FF17" s="1"/>
+      <c r="FG17" s="1"/>
+      <c r="FH17" s="1"/>
+      <c r="FI17" s="1"/>
+      <c r="FJ17" s="1"/>
+      <c r="FK17" s="1"/>
+      <c r="FL17" s="1"/>
+      <c r="FM17" s="1"/>
+      <c r="FN17" s="1"/>
+      <c r="FO17" s="1"/>
+      <c r="FP17" s="1"/>
+      <c r="FQ17" s="1"/>
+      <c r="FR17" s="1"/>
+      <c r="FS17" s="1"/>
+      <c r="FT17" s="1"/>
+      <c r="FU17" s="1"/>
+      <c r="FV17" s="1"/>
+      <c r="FW17" s="1"/>
+      <c r="FX17" s="1"/>
+      <c r="FY17" s="1"/>
+      <c r="FZ17" s="1"/>
+      <c r="GA17" s="1"/>
+      <c r="GB17" s="1"/>
+      <c r="GC17" s="1"/>
+      <c r="GD17" s="1"/>
+      <c r="GE17" s="1"/>
+      <c r="GF17" s="1"/>
+      <c r="GG17" s="1"/>
+      <c r="GH17" s="1"/>
+      <c r="GI17" s="1"/>
+      <c r="GJ17" s="1"/>
+      <c r="GK17" s="1"/>
+      <c r="GL17" s="1"/>
+      <c r="GM17" s="1"/>
+      <c r="GN17" s="1"/>
+      <c r="GO17" s="1"/>
+      <c r="GP17" s="1"/>
+      <c r="GQ17" s="1"/>
+      <c r="GR17" s="1"/>
+      <c r="GS17" s="1"/>
+      <c r="GT17" s="1"/>
+      <c r="GU17" s="1"/>
+      <c r="GV17" s="1"/>
+      <c r="GW17" s="1"/>
+      <c r="GX17" s="1"/>
+      <c r="GY17" s="1"/>
+      <c r="GZ17" s="1"/>
+      <c r="HA17" s="1"/>
+      <c r="HB17" s="1"/>
+      <c r="HC17" s="1"/>
+      <c r="HD17" s="1"/>
+      <c r="HE17" s="1"/>
+      <c r="HF17" s="1"/>
+      <c r="HG17" s="1"/>
+      <c r="HH17" s="1"/>
+      <c r="HI17" s="1"/>
+      <c r="HJ17" s="1"/>
+      <c r="HK17" s="1"/>
+      <c r="HL17" s="1"/>
+      <c r="HM17" s="1"/>
+      <c r="HN17" s="1"/>
+      <c r="HO17" s="1"/>
+      <c r="HP17" s="1"/>
+      <c r="HQ17" s="1"/>
+      <c r="HR17" s="1"/>
+      <c r="HS17" s="1"/>
+      <c r="HT17" s="1"/>
+      <c r="HU17" s="1"/>
+      <c r="HV17" s="1"/>
+      <c r="HW17" s="1"/>
+      <c r="HX17" s="1"/>
+      <c r="HY17" s="1"/>
+      <c r="HZ17" s="1"/>
+      <c r="IA17" s="1"/>
+      <c r="IB17" s="1"/>
+      <c r="IC17" s="1"/>
+      <c r="ID17" s="1"/>
+      <c r="IE17" s="1"/>
+      <c r="IF17" s="1"/>
+      <c r="IG17" s="1"/>
+      <c r="IH17" s="1"/>
+      <c r="II17" s="1"/>
+      <c r="IJ17" s="1"/>
+      <c r="IK17" s="1"/>
+      <c r="IL17" s="1"/>
+      <c r="IM17" s="1"/>
+      <c r="IN17" s="1"/>
+      <c r="IO17" s="1"/>
+      <c r="IP17" s="1"/>
+      <c r="IQ17" s="1"/>
+      <c r="IR17" s="1"/>
+      <c r="IS17" s="1"/>
+      <c r="IT17" s="1"/>
+      <c r="IU17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:255" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4">
-        <f>SUM(F3:F16)</f>
-        <v>52.5</v>
-      </c>
-      <c r="G24" s="4">
-        <f>SUM(G3:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>7</v>
+    <row r="25" spans="1:255" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <f>SUM(E3:E17)</f>
+        <v>56.5</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>